<commit_message>
Item Handling Refactor - Items now store their rarity, type and basetype information directly to get a full view of when the item was made - Added some more default icons - Items can now have different icons based on the item type that was being chosen - Updated CrystalBuild to fix some minor data issues
</commit_message>
<xml_diff>
--- a/data/content/ArmorNames.xlsx
+++ b/data/content/ArmorNames.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\EndlessBattleFC\data\content\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="18000" windowHeight="18240"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="18000" windowHeight="18240" firstSheet="5" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="ArmorNames_head" sheetId="9" r:id="rId1"/>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="72">
   <si>
     <t>Cap</t>
   </si>
@@ -239,6 +244,12 @@
   </si>
   <si>
     <t>Gadget</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>icon</t>
   </si>
 </sst>
 </file>
@@ -548,7 +559,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -556,67 +567,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -624,24 +679,37 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q40" sqref="Q40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -649,29 +717,148 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -679,84 +866,37 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -764,44 +904,52 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -809,29 +957,57 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -839,44 +1015,72 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -884,49 +1088,47 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -934,143 +1136,46 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>